<commit_message>
Added CreateWhatifScenarios and RemoveWhatifScenarios tests
</commit_message>
<xml_diff>
--- a/CreateWhatIfScenarios/Default.xlsx
+++ b/CreateWhatIfScenarios/Default.xlsx
@@ -14,6 +14,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+  <si>
+    <t>Current Plan</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>currentPortfolio</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>Full Pipeline</t>
+  </si>
+  <si>
+    <t>Black Diamond Scenario</t>
+  </si>
+  <si>
+    <t>2 Year Plan</t>
+  </si>
+  <si>
+    <t>RPAOS API TeamJoseph Banks_ Row 1 Col 1_out</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
@@ -154,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,13 +194,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -467,16 +529,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.4453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.71875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.41796875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -492,7 +613,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>

</xml_diff>

<commit_message>
Cleanup Whatif & added back change alm pw directory
</commit_message>
<xml_diff>
--- a/CreateWhatIfScenarios/Default.xlsx
+++ b/CreateWhatIfScenarios/Default.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="Action1" sheetId="2" r:id="rId2"/>
+    <sheet name="20 - Action" sheetId="2" r:id="rId2"/>
+    <sheet name="10 - Login" sheetId="3" r:id="rId3"/>
+    <sheet name="30 - Logout" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -224,10 +226,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
@@ -537,11 +539,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="20.4453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.71875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.41796875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.4453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.71875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.41796875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customFormat="1">
@@ -559,43 +561,43 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="3"/>
     </row>
   </sheetData>
@@ -604,6 +606,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.95"/>
+  <cols>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -611,9 +651,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>

</xml_diff>